<commit_message>
Visual Materials for section 2.2 and 2.1 are prepared and added to report.
</commit_message>
<xml_diff>
--- a/Course Materials/BinaryDom-ConceptEva.xlsx
+++ b/Course Materials/BinaryDom-ConceptEva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belgelerim\OneDrive\Masaüstü\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belgelerim\OneDrive\Masaüstü\FinalProject\Course Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -608,6 +608,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -629,12 +644,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -647,7 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -657,25 +666,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -708,9 +711,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -729,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -748,6 +748,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,6 +779,1391 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="tr-TR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-60F6-47A0-81CA-063C14E3C880}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3294686154981518E-2"/>
+                  <c:y val="-2.3221311532361569E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.2196457436654347E-2"/>
+                  <c:y val="-4.1798360758250809E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6736415829771867E-2"/>
+                  <c:y val="-5.9973629714597972E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3783838705509666E-2"/>
+                  <c:y val="-5.4648488430008253E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9421900257072553E-2"/>
+                  <c:y val="-9.2885246129447048E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.6069243334563315E-2"/>
+                  <c:y val="-4.6442623064723099E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6647343077490759E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6647343077490759E-2"/>
+                  <c:y val="1.857704922588924E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5491143591635868E-3"/>
+                  <c:y val="-2.3221311532361549E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3872785897908966E-2"/>
+                  <c:y val="-9.2885246129446614E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5491143591635868E-3"/>
+                  <c:y val="-1.3932786919416929E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-60F6-47A0-81CA-063C14E3C880}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sayfa1!$B$3:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Size-Restriction</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weight</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Control Stability</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Aesthetic</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Material Cost</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Manufacturability</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Reliability</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Noise</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Unusable-Rotor</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Transition Capability</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Hover Efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sayfa1!$P$3:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4.5454545454545456E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5151515151515152E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10606060606060606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.575757575757576E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13636363636363635</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15151515151515152</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0606060606060608E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0303030303030304E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12121212121212122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-60F6-47A0-81CA-063C14E3C880}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>98324</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>18436</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104467</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1031,8 +2431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="124" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,663 +2446,663 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="39" t="s">
+      <c r="C2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="47">
-        <v>1</v>
-      </c>
-      <c r="E3" s="48">
-        <v>0</v>
-      </c>
-      <c r="F3" s="48">
-        <v>0</v>
-      </c>
-      <c r="G3" s="48">
-        <v>0</v>
-      </c>
-      <c r="H3" s="48">
-        <v>0</v>
-      </c>
-      <c r="I3" s="48">
-        <v>0</v>
-      </c>
-      <c r="J3" s="48">
-        <v>0</v>
-      </c>
-      <c r="K3" s="48">
-        <v>1</v>
-      </c>
-      <c r="L3" s="48">
-        <v>0</v>
-      </c>
-      <c r="M3" s="48">
-        <v>1</v>
-      </c>
-      <c r="N3" s="49">
-        <v>0</v>
-      </c>
-      <c r="O3" s="41">
+      <c r="D3" s="42">
+        <v>1</v>
+      </c>
+      <c r="E3" s="43">
+        <v>0</v>
+      </c>
+      <c r="F3" s="43">
+        <v>0</v>
+      </c>
+      <c r="G3" s="43">
+        <v>0</v>
+      </c>
+      <c r="H3" s="43">
+        <v>0</v>
+      </c>
+      <c r="I3" s="43">
+        <v>0</v>
+      </c>
+      <c r="J3" s="43">
+        <v>0</v>
+      </c>
+      <c r="K3" s="43">
+        <v>1</v>
+      </c>
+      <c r="L3" s="43">
+        <v>0</v>
+      </c>
+      <c r="M3" s="43">
+        <v>1</v>
+      </c>
+      <c r="N3" s="44">
+        <v>0</v>
+      </c>
+      <c r="O3" s="36">
         <f>SUM(C3:N3)</f>
         <v>3</v>
       </c>
-      <c r="P3" s="42">
+      <c r="P3" s="37">
         <f>O3/66</f>
         <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="47">
-        <v>0</v>
-      </c>
-      <c r="D4" s="47" t="s">
+      <c r="B4" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="42">
+        <v>0</v>
+      </c>
+      <c r="D4" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="48">
-        <v>0</v>
-      </c>
-      <c r="F4" s="48">
-        <v>0</v>
-      </c>
-      <c r="G4" s="48">
-        <v>0</v>
-      </c>
-      <c r="H4" s="48">
-        <v>0</v>
-      </c>
-      <c r="I4" s="48">
-        <v>0</v>
-      </c>
-      <c r="J4" s="48">
-        <v>0</v>
-      </c>
-      <c r="K4" s="48">
-        <v>1</v>
-      </c>
-      <c r="L4" s="48">
-        <v>0</v>
-      </c>
-      <c r="M4" s="48">
-        <v>0</v>
-      </c>
-      <c r="N4" s="49">
-        <v>0</v>
-      </c>
-      <c r="O4" s="41">
+      <c r="E4" s="43">
+        <v>0</v>
+      </c>
+      <c r="F4" s="43">
+        <v>0</v>
+      </c>
+      <c r="G4" s="43">
+        <v>0</v>
+      </c>
+      <c r="H4" s="43">
+        <v>0</v>
+      </c>
+      <c r="I4" s="43">
+        <v>0</v>
+      </c>
+      <c r="J4" s="43">
+        <v>0</v>
+      </c>
+      <c r="K4" s="43">
+        <v>1</v>
+      </c>
+      <c r="L4" s="43">
+        <v>0</v>
+      </c>
+      <c r="M4" s="43">
+        <v>0</v>
+      </c>
+      <c r="N4" s="44">
+        <v>0</v>
+      </c>
+      <c r="O4" s="36">
         <f>SUM(C4:N4)</f>
         <v>1</v>
       </c>
-      <c r="P4" s="42">
+      <c r="P4" s="37">
         <f t="shared" ref="P4:P14" si="0">O4/66</f>
         <v>1.5151515151515152E-2</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="47">
-        <v>1</v>
-      </c>
-      <c r="D5" s="47">
-        <v>1</v>
-      </c>
-      <c r="E5" s="48" t="s">
+      <c r="C5" s="42">
+        <v>1</v>
+      </c>
+      <c r="D5" s="42">
+        <v>1</v>
+      </c>
+      <c r="E5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="48">
-        <v>0</v>
-      </c>
-      <c r="G5" s="48">
-        <v>1</v>
-      </c>
-      <c r="H5" s="48">
-        <v>1</v>
-      </c>
-      <c r="I5" s="48">
-        <v>0</v>
-      </c>
-      <c r="J5" s="48">
-        <v>0</v>
-      </c>
-      <c r="K5" s="48">
-        <v>1</v>
-      </c>
-      <c r="L5" s="48">
-        <v>1</v>
-      </c>
-      <c r="M5" s="48">
-        <v>1</v>
-      </c>
-      <c r="N5" s="49">
-        <v>0</v>
-      </c>
-      <c r="O5" s="41">
+      <c r="F5" s="43">
+        <v>0</v>
+      </c>
+      <c r="G5" s="43">
+        <v>1</v>
+      </c>
+      <c r="H5" s="43">
+        <v>1</v>
+      </c>
+      <c r="I5" s="43">
+        <v>0</v>
+      </c>
+      <c r="J5" s="43">
+        <v>0</v>
+      </c>
+      <c r="K5" s="43">
+        <v>1</v>
+      </c>
+      <c r="L5" s="43">
+        <v>1</v>
+      </c>
+      <c r="M5" s="43">
+        <v>1</v>
+      </c>
+      <c r="N5" s="44">
+        <v>0</v>
+      </c>
+      <c r="O5" s="36">
         <f>SUM(C5:N5)</f>
         <v>7</v>
       </c>
-      <c r="P5" s="42">
+      <c r="P5" s="37">
         <f t="shared" si="0"/>
         <v>0.10606060606060606</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="47">
-        <v>1</v>
-      </c>
-      <c r="D6" s="47">
-        <v>1</v>
-      </c>
-      <c r="E6" s="48">
-        <v>1</v>
-      </c>
-      <c r="F6" s="48" t="s">
+      <c r="C6" s="42">
+        <v>1</v>
+      </c>
+      <c r="D6" s="42">
+        <v>1</v>
+      </c>
+      <c r="E6" s="43">
+        <v>1</v>
+      </c>
+      <c r="F6" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="48">
-        <v>1</v>
-      </c>
-      <c r="H6" s="48">
-        <v>1</v>
-      </c>
-      <c r="I6" s="48">
-        <v>1</v>
-      </c>
-      <c r="J6" s="48">
-        <v>1</v>
-      </c>
-      <c r="K6" s="48">
-        <v>1</v>
-      </c>
-      <c r="L6" s="48">
-        <v>1</v>
-      </c>
-      <c r="M6" s="48">
-        <v>1</v>
-      </c>
-      <c r="N6" s="49">
-        <v>1</v>
-      </c>
-      <c r="O6" s="41">
+      <c r="G6" s="43">
+        <v>1</v>
+      </c>
+      <c r="H6" s="43">
+        <v>1</v>
+      </c>
+      <c r="I6" s="43">
+        <v>1</v>
+      </c>
+      <c r="J6" s="43">
+        <v>1</v>
+      </c>
+      <c r="K6" s="43">
+        <v>1</v>
+      </c>
+      <c r="L6" s="43">
+        <v>1</v>
+      </c>
+      <c r="M6" s="43">
+        <v>1</v>
+      </c>
+      <c r="N6" s="44">
+        <v>1</v>
+      </c>
+      <c r="O6" s="36">
         <f>SUM(C6:N6)</f>
         <v>11</v>
       </c>
-      <c r="P6" s="42">
+      <c r="P6" s="37">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="47">
-        <v>1</v>
-      </c>
-      <c r="D7" s="47">
-        <v>1</v>
-      </c>
-      <c r="E7" s="48">
-        <v>0</v>
-      </c>
-      <c r="F7" s="48">
-        <v>0</v>
-      </c>
-      <c r="G7" s="48" t="s">
+      <c r="C7" s="42">
+        <v>1</v>
+      </c>
+      <c r="D7" s="42">
+        <v>1</v>
+      </c>
+      <c r="E7" s="43">
+        <v>0</v>
+      </c>
+      <c r="F7" s="43">
+        <v>0</v>
+      </c>
+      <c r="G7" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="48">
-        <v>1</v>
-      </c>
-      <c r="I7" s="48">
-        <v>0</v>
-      </c>
-      <c r="J7" s="48">
-        <v>0</v>
-      </c>
-      <c r="K7" s="48">
-        <v>1</v>
-      </c>
-      <c r="L7" s="48">
-        <v>1</v>
-      </c>
-      <c r="M7" s="48">
-        <v>1</v>
-      </c>
-      <c r="N7" s="49">
-        <v>0</v>
-      </c>
-      <c r="O7" s="41">
+      <c r="H7" s="43">
+        <v>1</v>
+      </c>
+      <c r="I7" s="43">
+        <v>0</v>
+      </c>
+      <c r="J7" s="43">
+        <v>0</v>
+      </c>
+      <c r="K7" s="43">
+        <v>1</v>
+      </c>
+      <c r="L7" s="43">
+        <v>1</v>
+      </c>
+      <c r="M7" s="43">
+        <v>1</v>
+      </c>
+      <c r="N7" s="44">
+        <v>0</v>
+      </c>
+      <c r="O7" s="36">
         <f t="shared" ref="O7:O14" si="1">SUM(C7:N7)</f>
         <v>6</v>
       </c>
-      <c r="P7" s="42">
+      <c r="P7" s="37">
         <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="47">
-        <v>1</v>
-      </c>
-      <c r="D8" s="47">
-        <v>1</v>
-      </c>
-      <c r="E8" s="48">
-        <v>0</v>
-      </c>
-      <c r="F8" s="48">
-        <v>0</v>
-      </c>
-      <c r="G8" s="48">
-        <v>0</v>
-      </c>
-      <c r="H8" s="48" t="s">
+      <c r="C8" s="42">
+        <v>1</v>
+      </c>
+      <c r="D8" s="42">
+        <v>1</v>
+      </c>
+      <c r="E8" s="43">
+        <v>0</v>
+      </c>
+      <c r="F8" s="43">
+        <v>0</v>
+      </c>
+      <c r="G8" s="43">
+        <v>0</v>
+      </c>
+      <c r="H8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="48">
-        <v>0</v>
-      </c>
-      <c r="J8" s="48">
-        <v>0</v>
-      </c>
-      <c r="K8" s="48">
-        <v>1</v>
-      </c>
-      <c r="L8" s="48">
-        <v>1</v>
-      </c>
-      <c r="M8" s="48">
-        <v>1</v>
-      </c>
-      <c r="N8" s="49">
-        <v>0</v>
-      </c>
-      <c r="O8" s="41">
+      <c r="I8" s="43">
+        <v>0</v>
+      </c>
+      <c r="J8" s="43">
+        <v>0</v>
+      </c>
+      <c r="K8" s="43">
+        <v>1</v>
+      </c>
+      <c r="L8" s="43">
+        <v>1</v>
+      </c>
+      <c r="M8" s="43">
+        <v>1</v>
+      </c>
+      <c r="N8" s="44">
+        <v>0</v>
+      </c>
+      <c r="O8" s="36">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="P8" s="42">
+      <c r="P8" s="37">
         <f t="shared" si="0"/>
         <v>7.575757575757576E-2</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="47">
-        <v>1</v>
-      </c>
-      <c r="D9" s="47">
-        <v>1</v>
-      </c>
-      <c r="E9" s="48">
-        <v>1</v>
-      </c>
-      <c r="F9" s="48">
-        <v>0</v>
-      </c>
-      <c r="G9" s="48">
-        <v>1</v>
-      </c>
-      <c r="H9" s="48">
-        <v>1</v>
-      </c>
-      <c r="I9" s="48" t="s">
+      <c r="C9" s="42">
+        <v>1</v>
+      </c>
+      <c r="D9" s="42">
+        <v>1</v>
+      </c>
+      <c r="E9" s="43">
+        <v>1</v>
+      </c>
+      <c r="F9" s="43">
+        <v>0</v>
+      </c>
+      <c r="G9" s="43">
+        <v>1</v>
+      </c>
+      <c r="H9" s="43">
+        <v>1</v>
+      </c>
+      <c r="I9" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="48">
-        <v>0</v>
-      </c>
-      <c r="K9" s="48">
-        <v>1</v>
-      </c>
-      <c r="L9" s="48">
-        <v>1</v>
-      </c>
-      <c r="M9" s="48">
-        <v>1</v>
-      </c>
-      <c r="N9" s="49">
-        <v>1</v>
-      </c>
-      <c r="O9" s="41">
+      <c r="J9" s="43">
+        <v>0</v>
+      </c>
+      <c r="K9" s="43">
+        <v>1</v>
+      </c>
+      <c r="L9" s="43">
+        <v>1</v>
+      </c>
+      <c r="M9" s="43">
+        <v>1</v>
+      </c>
+      <c r="N9" s="44">
+        <v>1</v>
+      </c>
+      <c r="O9" s="36">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="37">
         <f t="shared" si="0"/>
         <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="47">
-        <v>1</v>
-      </c>
-      <c r="D10" s="47">
-        <v>1</v>
-      </c>
-      <c r="E10" s="48">
-        <v>1</v>
-      </c>
-      <c r="F10" s="48">
-        <v>0</v>
-      </c>
-      <c r="G10" s="48">
-        <v>1</v>
-      </c>
-      <c r="H10" s="48">
-        <v>1</v>
-      </c>
-      <c r="I10" s="48">
-        <v>1</v>
-      </c>
-      <c r="J10" s="48" t="s">
+      <c r="C10" s="42">
+        <v>1</v>
+      </c>
+      <c r="D10" s="42">
+        <v>1</v>
+      </c>
+      <c r="E10" s="43">
+        <v>1</v>
+      </c>
+      <c r="F10" s="43">
+        <v>0</v>
+      </c>
+      <c r="G10" s="43">
+        <v>1</v>
+      </c>
+      <c r="H10" s="43">
+        <v>1</v>
+      </c>
+      <c r="I10" s="43">
+        <v>1</v>
+      </c>
+      <c r="J10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="48">
-        <v>1</v>
-      </c>
-      <c r="L10" s="48">
-        <v>1</v>
-      </c>
-      <c r="M10" s="48">
-        <v>1</v>
-      </c>
-      <c r="N10" s="49">
-        <v>1</v>
-      </c>
-      <c r="O10" s="41">
+      <c r="K10" s="43">
+        <v>1</v>
+      </c>
+      <c r="L10" s="43">
+        <v>1</v>
+      </c>
+      <c r="M10" s="43">
+        <v>1</v>
+      </c>
+      <c r="N10" s="44">
+        <v>1</v>
+      </c>
+      <c r="O10" s="36">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="P10" s="42">
+      <c r="P10" s="37">
         <f t="shared" si="0"/>
         <v>0.15151515151515152</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="47">
-        <v>0</v>
-      </c>
-      <c r="D11" s="47">
-        <v>0</v>
-      </c>
-      <c r="E11" s="48">
-        <v>0</v>
-      </c>
-      <c r="F11" s="48">
-        <v>0</v>
-      </c>
-      <c r="G11" s="48">
-        <v>0</v>
-      </c>
-      <c r="H11" s="48">
-        <v>0</v>
-      </c>
-      <c r="I11" s="48">
-        <v>0</v>
-      </c>
-      <c r="J11" s="48">
-        <v>0</v>
-      </c>
-      <c r="K11" s="48" t="s">
+      <c r="C11" s="42">
+        <v>0</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="43">
+        <v>0</v>
+      </c>
+      <c r="F11" s="43">
+        <v>0</v>
+      </c>
+      <c r="G11" s="43">
+        <v>0</v>
+      </c>
+      <c r="H11" s="43">
+        <v>0</v>
+      </c>
+      <c r="I11" s="43">
+        <v>0</v>
+      </c>
+      <c r="J11" s="43">
+        <v>0</v>
+      </c>
+      <c r="K11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="48">
-        <v>0</v>
-      </c>
-      <c r="M11" s="48">
-        <v>0</v>
-      </c>
-      <c r="N11" s="49">
-        <v>0</v>
-      </c>
-      <c r="O11" s="41">
+      <c r="L11" s="43">
+        <v>0</v>
+      </c>
+      <c r="M11" s="43">
+        <v>0</v>
+      </c>
+      <c r="N11" s="44">
+        <v>0</v>
+      </c>
+      <c r="O11" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P11" s="42">
+      <c r="P11" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="47">
-        <v>1</v>
-      </c>
-      <c r="D12" s="47">
-        <v>1</v>
-      </c>
-      <c r="E12" s="48">
-        <v>0</v>
-      </c>
-      <c r="F12" s="48">
-        <v>0</v>
-      </c>
-      <c r="G12" s="48">
-        <v>0</v>
-      </c>
-      <c r="H12" s="48">
-        <v>0</v>
-      </c>
-      <c r="I12" s="48">
-        <v>0</v>
-      </c>
-      <c r="J12" s="48">
-        <v>0</v>
-      </c>
-      <c r="K12" s="48">
-        <v>1</v>
-      </c>
-      <c r="L12" s="48" t="s">
+      <c r="C12" s="42">
+        <v>1</v>
+      </c>
+      <c r="D12" s="42">
+        <v>1</v>
+      </c>
+      <c r="E12" s="43">
+        <v>0</v>
+      </c>
+      <c r="F12" s="43">
+        <v>0</v>
+      </c>
+      <c r="G12" s="43">
+        <v>0</v>
+      </c>
+      <c r="H12" s="43">
+        <v>0</v>
+      </c>
+      <c r="I12" s="43">
+        <v>0</v>
+      </c>
+      <c r="J12" s="43">
+        <v>0</v>
+      </c>
+      <c r="K12" s="43">
+        <v>1</v>
+      </c>
+      <c r="L12" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="48">
-        <v>1</v>
-      </c>
-      <c r="N12" s="49">
-        <v>0</v>
-      </c>
-      <c r="O12" s="41">
+      <c r="M12" s="43">
+        <v>1</v>
+      </c>
+      <c r="N12" s="44">
+        <v>0</v>
+      </c>
+      <c r="O12" s="36">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="P12" s="42">
+      <c r="P12" s="37">
         <f t="shared" si="0"/>
         <v>6.0606060606060608E-2</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="47">
-        <v>0</v>
-      </c>
-      <c r="D13" s="47">
-        <v>1</v>
-      </c>
-      <c r="E13" s="48">
-        <v>0</v>
-      </c>
-      <c r="F13" s="48">
-        <v>0</v>
-      </c>
-      <c r="G13" s="48">
-        <v>0</v>
-      </c>
-      <c r="H13" s="48">
-        <v>0</v>
-      </c>
-      <c r="I13" s="48">
-        <v>0</v>
-      </c>
-      <c r="J13" s="48">
-        <v>0</v>
-      </c>
-      <c r="K13" s="48">
-        <v>1</v>
-      </c>
-      <c r="L13" s="48">
-        <v>0</v>
-      </c>
-      <c r="M13" s="48" t="s">
+      <c r="C13" s="42">
+        <v>0</v>
+      </c>
+      <c r="D13" s="42">
+        <v>1</v>
+      </c>
+      <c r="E13" s="43">
+        <v>0</v>
+      </c>
+      <c r="F13" s="43">
+        <v>0</v>
+      </c>
+      <c r="G13" s="43">
+        <v>0</v>
+      </c>
+      <c r="H13" s="43">
+        <v>0</v>
+      </c>
+      <c r="I13" s="43">
+        <v>0</v>
+      </c>
+      <c r="J13" s="43">
+        <v>0</v>
+      </c>
+      <c r="K13" s="43">
+        <v>1</v>
+      </c>
+      <c r="L13" s="43">
+        <v>0</v>
+      </c>
+      <c r="M13" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="N13" s="49">
-        <v>0</v>
-      </c>
-      <c r="O13" s="41">
+      <c r="N13" s="44">
+        <v>0</v>
+      </c>
+      <c r="O13" s="36">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="P13" s="42">
+      <c r="P13" s="37">
         <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="38">
-        <v>1</v>
-      </c>
-      <c r="D14" s="38">
-        <v>1</v>
-      </c>
-      <c r="E14" s="40">
-        <v>1</v>
-      </c>
-      <c r="F14" s="40">
-        <v>0</v>
-      </c>
-      <c r="G14" s="40">
-        <v>1</v>
-      </c>
-      <c r="H14" s="40">
-        <v>1</v>
-      </c>
-      <c r="I14" s="40">
-        <v>0</v>
-      </c>
-      <c r="J14" s="40">
-        <v>0</v>
-      </c>
-      <c r="K14" s="40">
-        <v>1</v>
-      </c>
-      <c r="L14" s="40">
-        <v>1</v>
-      </c>
-      <c r="M14" s="40">
-        <v>1</v>
-      </c>
-      <c r="N14" s="11" t="s">
+      <c r="C14" s="33">
+        <v>1</v>
+      </c>
+      <c r="D14" s="33">
+        <v>1</v>
+      </c>
+      <c r="E14" s="35">
+        <v>1</v>
+      </c>
+      <c r="F14" s="35">
+        <v>0</v>
+      </c>
+      <c r="G14" s="35">
+        <v>1</v>
+      </c>
+      <c r="H14" s="35">
+        <v>1</v>
+      </c>
+      <c r="I14" s="35">
+        <v>0</v>
+      </c>
+      <c r="J14" s="35">
+        <v>0</v>
+      </c>
+      <c r="K14" s="35">
+        <v>1</v>
+      </c>
+      <c r="L14" s="35">
+        <v>1</v>
+      </c>
+      <c r="M14" s="35">
+        <v>1</v>
+      </c>
+      <c r="N14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="10">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="12">
         <f t="shared" si="0"/>
         <v>0.12121212121212122</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="13">
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="11">
         <f>SUM(O3:O14)</f>
         <v>66</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="14">
         <f>SUM(P3:P14)</f>
         <v>1</v>
       </c>
@@ -1737,6 +3137,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1748,7 +3149,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="B2:F15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1761,41 +3162,41 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="18">
         <f>Sayfa1!P3</f>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="21">
         <v>70</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="21">
         <v>80</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="24">
         <v>50</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="6">
         <f>D3*C3</f>
         <v>3.1818181818181821</v>
@@ -1813,20 +3214,20 @@
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="19">
         <f>Sayfa1!P4</f>
         <v>1.5151515151515152E-2</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="22">
         <v>60</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="22">
         <v>50</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="25">
         <v>70</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="6">
         <f>D4*C4</f>
         <v>0.90909090909090917</v>
@@ -1844,20 +3245,20 @@
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="19">
         <f>Sayfa1!P5</f>
         <v>0.10606060606060606</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="22">
         <v>60</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="22">
         <v>40</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="25">
         <v>40</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="6">
         <f t="shared" ref="H5:H14" si="1">D5*C5</f>
         <v>6.3636363636363642</v>
@@ -1875,20 +3276,20 @@
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="19">
         <f>Sayfa1!P6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="22">
         <v>70</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="22">
         <v>80</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="25">
         <v>30</v>
       </c>
-      <c r="G6" s="17"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="6">
         <f t="shared" si="1"/>
         <v>11.666666666666666</v>
@@ -1906,20 +3307,20 @@
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="19">
         <f>Sayfa1!P7</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="22">
         <v>80</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="22">
         <v>50</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="25">
         <v>60</v>
       </c>
-      <c r="G7" s="17"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="6">
         <f t="shared" si="1"/>
         <v>7.2727272727272734</v>
@@ -1937,20 +3338,20 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="19">
         <f>Sayfa1!P8</f>
         <v>7.575757575757576E-2</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="22">
         <v>75</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="22">
         <v>70</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="25">
         <v>80</v>
       </c>
-      <c r="G8" s="17"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="6">
         <f t="shared" si="1"/>
         <v>5.6818181818181817</v>
@@ -1968,20 +3369,20 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="19">
         <f>Sayfa1!P9</f>
         <v>0.13636363636363635</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="22">
         <v>65</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="22">
         <v>55</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="25">
         <v>50</v>
       </c>
-      <c r="G9" s="17"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
         <v>8.8636363636363633</v>
@@ -1999,20 +3400,20 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="19">
         <f>Sayfa1!P10</f>
         <v>0.15151515151515152</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="22">
         <v>50</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="22">
         <v>60</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="25">
         <v>30</v>
       </c>
-      <c r="G10" s="17"/>
+      <c r="G10" s="15"/>
       <c r="H10" s="6">
         <f t="shared" si="1"/>
         <v>7.5757575757575761</v>
@@ -2030,20 +3431,20 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="19">
         <f>Sayfa1!P11</f>
         <v>0</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="22">
         <v>40</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="22">
         <v>30</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="25">
         <v>50</v>
       </c>
-      <c r="G11" s="17"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2061,20 +3462,20 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="19">
         <f>Sayfa1!P12</f>
         <v>6.0606060606060608E-2</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="22">
         <v>60</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="22">
         <v>30</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="25">
         <v>90</v>
       </c>
-      <c r="G12" s="17"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="6">
         <f t="shared" si="1"/>
         <v>3.6363636363636367</v>
@@ -2092,20 +3493,20 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="19">
         <f>Sayfa1!P13</f>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="22">
         <v>60</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="22">
         <v>60</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="25">
         <v>30</v>
       </c>
-      <c r="G13" s="17"/>
+      <c r="G13" s="15"/>
       <c r="H13" s="6">
         <f t="shared" si="1"/>
         <v>1.8181818181818183</v>
@@ -2123,20 +3524,20 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="20">
         <f>Sayfa1!P14</f>
         <v>0.12121212121212122</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="23">
         <v>70</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="23">
         <v>80</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="26">
         <v>60</v>
       </c>
-      <c r="G14" s="17"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="6">
         <f t="shared" si="1"/>
         <v>8.4848484848484844</v>
@@ -2151,47 +3552,47 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="33">
+      <c r="C15" s="49"/>
+      <c r="D15" s="29">
         <f>SUM(H3:H14)</f>
         <v>65.454545454545467</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="28">
         <f>SUM(I3:I14)</f>
         <v>61.742424242424249</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="27">
         <f>SUM(J3:J14)</f>
         <v>49.090909090909086</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Report 2.2 is finalised.
</commit_message>
<xml_diff>
--- a/Course Materials/BinaryDom-ConceptEva.xlsx
+++ b/Course Materials/BinaryDom-ConceptEva.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +169,16 @@
       <family val="1"/>
       <charset val="162"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +189,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -624,8 +637,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -702,9 +716,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,8 +775,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="İyi" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1252,9 +1267,7 @@
               <c:idx val="8"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-60F6-47A0-81CA-063C14E3C880}"/>
                 </c:ext>
@@ -1384,9 +1397,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2431,7 +2442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="124" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="124" workbookViewId="0">
       <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
@@ -2446,40 +2457,40 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="34" t="s">
+      <c r="C2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="33" t="s">
         <v>10</v>
       </c>
       <c r="N2" s="8" t="s">
@@ -2495,579 +2506,579 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="42">
-        <v>1</v>
-      </c>
-      <c r="E3" s="43">
-        <v>0</v>
-      </c>
-      <c r="F3" s="43">
-        <v>0</v>
-      </c>
-      <c r="G3" s="43">
-        <v>0</v>
-      </c>
-      <c r="H3" s="43">
-        <v>0</v>
-      </c>
-      <c r="I3" s="43">
-        <v>0</v>
-      </c>
-      <c r="J3" s="43">
-        <v>0</v>
-      </c>
-      <c r="K3" s="43">
-        <v>1</v>
-      </c>
-      <c r="L3" s="43">
-        <v>0</v>
-      </c>
-      <c r="M3" s="43">
-        <v>1</v>
-      </c>
-      <c r="N3" s="44">
-        <v>0</v>
-      </c>
-      <c r="O3" s="36">
+      <c r="D3" s="41">
+        <v>1</v>
+      </c>
+      <c r="E3" s="42">
+        <v>0</v>
+      </c>
+      <c r="F3" s="42">
+        <v>0</v>
+      </c>
+      <c r="G3" s="42">
+        <v>0</v>
+      </c>
+      <c r="H3" s="42">
+        <v>0</v>
+      </c>
+      <c r="I3" s="42">
+        <v>0</v>
+      </c>
+      <c r="J3" s="42">
+        <v>0</v>
+      </c>
+      <c r="K3" s="42">
+        <v>1</v>
+      </c>
+      <c r="L3" s="42">
+        <v>0</v>
+      </c>
+      <c r="M3" s="42">
+        <v>1</v>
+      </c>
+      <c r="N3" s="43">
+        <v>0</v>
+      </c>
+      <c r="O3" s="35">
         <f>SUM(C3:N3)</f>
         <v>3</v>
       </c>
-      <c r="P3" s="37">
+      <c r="P3" s="36">
         <f>O3/66</f>
         <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42">
-        <v>0</v>
-      </c>
-      <c r="D4" s="42" t="s">
+      <c r="B4" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0</v>
+      </c>
+      <c r="D4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="43">
-        <v>0</v>
-      </c>
-      <c r="F4" s="43">
-        <v>0</v>
-      </c>
-      <c r="G4" s="43">
-        <v>0</v>
-      </c>
-      <c r="H4" s="43">
-        <v>0</v>
-      </c>
-      <c r="I4" s="43">
-        <v>0</v>
-      </c>
-      <c r="J4" s="43">
-        <v>0</v>
-      </c>
-      <c r="K4" s="43">
-        <v>1</v>
-      </c>
-      <c r="L4" s="43">
-        <v>0</v>
-      </c>
-      <c r="M4" s="43">
-        <v>0</v>
-      </c>
-      <c r="N4" s="44">
-        <v>0</v>
-      </c>
-      <c r="O4" s="36">
+      <c r="E4" s="42">
+        <v>0</v>
+      </c>
+      <c r="F4" s="42">
+        <v>0</v>
+      </c>
+      <c r="G4" s="42">
+        <v>0</v>
+      </c>
+      <c r="H4" s="42">
+        <v>0</v>
+      </c>
+      <c r="I4" s="42">
+        <v>0</v>
+      </c>
+      <c r="J4" s="42">
+        <v>0</v>
+      </c>
+      <c r="K4" s="42">
+        <v>1</v>
+      </c>
+      <c r="L4" s="42">
+        <v>0</v>
+      </c>
+      <c r="M4" s="42">
+        <v>0</v>
+      </c>
+      <c r="N4" s="43">
+        <v>0</v>
+      </c>
+      <c r="O4" s="35">
         <f>SUM(C4:N4)</f>
         <v>1</v>
       </c>
-      <c r="P4" s="37">
+      <c r="P4" s="36">
         <f t="shared" ref="P4:P14" si="0">O4/66</f>
         <v>1.5151515151515152E-2</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="42">
-        <v>1</v>
-      </c>
-      <c r="E5" s="43" t="s">
+      <c r="C5" s="41">
+        <v>1</v>
+      </c>
+      <c r="D5" s="41">
+        <v>1</v>
+      </c>
+      <c r="E5" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="43">
-        <v>0</v>
-      </c>
-      <c r="G5" s="43">
-        <v>1</v>
-      </c>
-      <c r="H5" s="43">
-        <v>1</v>
-      </c>
-      <c r="I5" s="43">
-        <v>0</v>
-      </c>
-      <c r="J5" s="43">
-        <v>0</v>
-      </c>
-      <c r="K5" s="43">
-        <v>1</v>
-      </c>
-      <c r="L5" s="43">
-        <v>1</v>
-      </c>
-      <c r="M5" s="43">
-        <v>1</v>
-      </c>
-      <c r="N5" s="44">
-        <v>0</v>
-      </c>
-      <c r="O5" s="36">
+      <c r="F5" s="42">
+        <v>0</v>
+      </c>
+      <c r="G5" s="42">
+        <v>1</v>
+      </c>
+      <c r="H5" s="42">
+        <v>1</v>
+      </c>
+      <c r="I5" s="42">
+        <v>0</v>
+      </c>
+      <c r="J5" s="42">
+        <v>0</v>
+      </c>
+      <c r="K5" s="42">
+        <v>1</v>
+      </c>
+      <c r="L5" s="42">
+        <v>1</v>
+      </c>
+      <c r="M5" s="42">
+        <v>1</v>
+      </c>
+      <c r="N5" s="43">
+        <v>0</v>
+      </c>
+      <c r="O5" s="35">
         <f>SUM(C5:N5)</f>
         <v>7</v>
       </c>
-      <c r="P5" s="37">
+      <c r="P5" s="36">
         <f t="shared" si="0"/>
         <v>0.10606060606060606</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="42">
-        <v>1</v>
-      </c>
-      <c r="E6" s="43">
-        <v>1</v>
-      </c>
-      <c r="F6" s="43" t="s">
+      <c r="C6" s="41">
+        <v>1</v>
+      </c>
+      <c r="D6" s="41">
+        <v>1</v>
+      </c>
+      <c r="E6" s="42">
+        <v>1</v>
+      </c>
+      <c r="F6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="43">
-        <v>1</v>
-      </c>
-      <c r="H6" s="43">
-        <v>1</v>
-      </c>
-      <c r="I6" s="43">
-        <v>1</v>
-      </c>
-      <c r="J6" s="43">
-        <v>1</v>
-      </c>
-      <c r="K6" s="43">
-        <v>1</v>
-      </c>
-      <c r="L6" s="43">
-        <v>1</v>
-      </c>
-      <c r="M6" s="43">
-        <v>1</v>
-      </c>
-      <c r="N6" s="44">
-        <v>1</v>
-      </c>
-      <c r="O6" s="36">
+      <c r="G6" s="42">
+        <v>1</v>
+      </c>
+      <c r="H6" s="42">
+        <v>1</v>
+      </c>
+      <c r="I6" s="42">
+        <v>1</v>
+      </c>
+      <c r="J6" s="42">
+        <v>1</v>
+      </c>
+      <c r="K6" s="42">
+        <v>1</v>
+      </c>
+      <c r="L6" s="42">
+        <v>1</v>
+      </c>
+      <c r="M6" s="42">
+        <v>1</v>
+      </c>
+      <c r="N6" s="43">
+        <v>1</v>
+      </c>
+      <c r="O6" s="35">
         <f>SUM(C6:N6)</f>
         <v>11</v>
       </c>
-      <c r="P6" s="37">
+      <c r="P6" s="36">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="42">
-        <v>1</v>
-      </c>
-      <c r="D7" s="42">
-        <v>1</v>
-      </c>
-      <c r="E7" s="43">
-        <v>0</v>
-      </c>
-      <c r="F7" s="43">
-        <v>0</v>
-      </c>
-      <c r="G7" s="43" t="s">
+      <c r="C7" s="41">
+        <v>1</v>
+      </c>
+      <c r="D7" s="41">
+        <v>1</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0</v>
+      </c>
+      <c r="F7" s="42">
+        <v>0</v>
+      </c>
+      <c r="G7" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="43">
-        <v>1</v>
-      </c>
-      <c r="I7" s="43">
-        <v>0</v>
-      </c>
-      <c r="J7" s="43">
-        <v>0</v>
-      </c>
-      <c r="K7" s="43">
-        <v>1</v>
-      </c>
-      <c r="L7" s="43">
-        <v>1</v>
-      </c>
-      <c r="M7" s="43">
-        <v>1</v>
-      </c>
-      <c r="N7" s="44">
-        <v>0</v>
-      </c>
-      <c r="O7" s="36">
+      <c r="H7" s="42">
+        <v>1</v>
+      </c>
+      <c r="I7" s="42">
+        <v>0</v>
+      </c>
+      <c r="J7" s="42">
+        <v>0</v>
+      </c>
+      <c r="K7" s="42">
+        <v>1</v>
+      </c>
+      <c r="L7" s="42">
+        <v>1</v>
+      </c>
+      <c r="M7" s="42">
+        <v>1</v>
+      </c>
+      <c r="N7" s="43">
+        <v>0</v>
+      </c>
+      <c r="O7" s="35">
         <f t="shared" ref="O7:O14" si="1">SUM(C7:N7)</f>
         <v>6</v>
       </c>
-      <c r="P7" s="37">
+      <c r="P7" s="36">
         <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="D8" s="42">
-        <v>1</v>
-      </c>
-      <c r="E8" s="43">
-        <v>0</v>
-      </c>
-      <c r="F8" s="43">
-        <v>0</v>
-      </c>
-      <c r="G8" s="43">
-        <v>0</v>
-      </c>
-      <c r="H8" s="43" t="s">
+      <c r="C8" s="41">
+        <v>1</v>
+      </c>
+      <c r="D8" s="41">
+        <v>1</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0</v>
+      </c>
+      <c r="F8" s="42">
+        <v>0</v>
+      </c>
+      <c r="G8" s="42">
+        <v>0</v>
+      </c>
+      <c r="H8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="43">
-        <v>0</v>
-      </c>
-      <c r="J8" s="43">
-        <v>0</v>
-      </c>
-      <c r="K8" s="43">
-        <v>1</v>
-      </c>
-      <c r="L8" s="43">
-        <v>1</v>
-      </c>
-      <c r="M8" s="43">
-        <v>1</v>
-      </c>
-      <c r="N8" s="44">
-        <v>0</v>
-      </c>
-      <c r="O8" s="36">
+      <c r="I8" s="42">
+        <v>0</v>
+      </c>
+      <c r="J8" s="42">
+        <v>0</v>
+      </c>
+      <c r="K8" s="42">
+        <v>1</v>
+      </c>
+      <c r="L8" s="42">
+        <v>1</v>
+      </c>
+      <c r="M8" s="42">
+        <v>1</v>
+      </c>
+      <c r="N8" s="43">
+        <v>0</v>
+      </c>
+      <c r="O8" s="35">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="P8" s="37">
+      <c r="P8" s="36">
         <f t="shared" si="0"/>
         <v>7.575757575757576E-2</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="42">
-        <v>1</v>
-      </c>
-      <c r="D9" s="42">
-        <v>1</v>
-      </c>
-      <c r="E9" s="43">
-        <v>1</v>
-      </c>
-      <c r="F9" s="43">
-        <v>0</v>
-      </c>
-      <c r="G9" s="43">
-        <v>1</v>
-      </c>
-      <c r="H9" s="43">
-        <v>1</v>
-      </c>
-      <c r="I9" s="43" t="s">
+      <c r="C9" s="41">
+        <v>1</v>
+      </c>
+      <c r="D9" s="41">
+        <v>1</v>
+      </c>
+      <c r="E9" s="42">
+        <v>1</v>
+      </c>
+      <c r="F9" s="42">
+        <v>0</v>
+      </c>
+      <c r="G9" s="42">
+        <v>1</v>
+      </c>
+      <c r="H9" s="42">
+        <v>1</v>
+      </c>
+      <c r="I9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="43">
-        <v>0</v>
-      </c>
-      <c r="K9" s="43">
-        <v>1</v>
-      </c>
-      <c r="L9" s="43">
-        <v>1</v>
-      </c>
-      <c r="M9" s="43">
-        <v>1</v>
-      </c>
-      <c r="N9" s="44">
-        <v>1</v>
-      </c>
-      <c r="O9" s="36">
+      <c r="J9" s="42">
+        <v>0</v>
+      </c>
+      <c r="K9" s="42">
+        <v>1</v>
+      </c>
+      <c r="L9" s="42">
+        <v>1</v>
+      </c>
+      <c r="M9" s="42">
+        <v>1</v>
+      </c>
+      <c r="N9" s="43">
+        <v>1</v>
+      </c>
+      <c r="O9" s="35">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="P9" s="37">
+      <c r="P9" s="36">
         <f t="shared" si="0"/>
         <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="42">
-        <v>1</v>
-      </c>
-      <c r="D10" s="42">
-        <v>1</v>
-      </c>
-      <c r="E10" s="43">
-        <v>1</v>
-      </c>
-      <c r="F10" s="43">
-        <v>0</v>
-      </c>
-      <c r="G10" s="43">
-        <v>1</v>
-      </c>
-      <c r="H10" s="43">
-        <v>1</v>
-      </c>
-      <c r="I10" s="43">
-        <v>1</v>
-      </c>
-      <c r="J10" s="43" t="s">
+      <c r="C10" s="41">
+        <v>1</v>
+      </c>
+      <c r="D10" s="41">
+        <v>1</v>
+      </c>
+      <c r="E10" s="42">
+        <v>1</v>
+      </c>
+      <c r="F10" s="42">
+        <v>0</v>
+      </c>
+      <c r="G10" s="42">
+        <v>1</v>
+      </c>
+      <c r="H10" s="42">
+        <v>1</v>
+      </c>
+      <c r="I10" s="42">
+        <v>1</v>
+      </c>
+      <c r="J10" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="43">
-        <v>1</v>
-      </c>
-      <c r="L10" s="43">
-        <v>1</v>
-      </c>
-      <c r="M10" s="43">
-        <v>1</v>
-      </c>
-      <c r="N10" s="44">
-        <v>1</v>
-      </c>
-      <c r="O10" s="36">
+      <c r="K10" s="42">
+        <v>1</v>
+      </c>
+      <c r="L10" s="42">
+        <v>1</v>
+      </c>
+      <c r="M10" s="42">
+        <v>1</v>
+      </c>
+      <c r="N10" s="43">
+        <v>1</v>
+      </c>
+      <c r="O10" s="35">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="P10" s="37">
+      <c r="P10" s="36">
         <f t="shared" si="0"/>
         <v>0.15151515151515152</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="42">
-        <v>0</v>
-      </c>
-      <c r="D11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="43">
-        <v>0</v>
-      </c>
-      <c r="F11" s="43">
-        <v>0</v>
-      </c>
-      <c r="G11" s="43">
-        <v>0</v>
-      </c>
-      <c r="H11" s="43">
-        <v>0</v>
-      </c>
-      <c r="I11" s="43">
-        <v>0</v>
-      </c>
-      <c r="J11" s="43">
-        <v>0</v>
-      </c>
-      <c r="K11" s="43" t="s">
+      <c r="C11" s="41">
+        <v>0</v>
+      </c>
+      <c r="D11" s="41">
+        <v>0</v>
+      </c>
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="F11" s="42">
+        <v>0</v>
+      </c>
+      <c r="G11" s="42">
+        <v>0</v>
+      </c>
+      <c r="H11" s="42">
+        <v>0</v>
+      </c>
+      <c r="I11" s="42">
+        <v>0</v>
+      </c>
+      <c r="J11" s="42">
+        <v>0</v>
+      </c>
+      <c r="K11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="43">
-        <v>0</v>
-      </c>
-      <c r="M11" s="43">
-        <v>0</v>
-      </c>
-      <c r="N11" s="44">
-        <v>0</v>
-      </c>
-      <c r="O11" s="36">
+      <c r="L11" s="42">
+        <v>0</v>
+      </c>
+      <c r="M11" s="42">
+        <v>0</v>
+      </c>
+      <c r="N11" s="43">
+        <v>0</v>
+      </c>
+      <c r="O11" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P11" s="37">
+      <c r="P11" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="42">
-        <v>1</v>
-      </c>
-      <c r="D12" s="42">
-        <v>1</v>
-      </c>
-      <c r="E12" s="43">
-        <v>0</v>
-      </c>
-      <c r="F12" s="43">
-        <v>0</v>
-      </c>
-      <c r="G12" s="43">
-        <v>0</v>
-      </c>
-      <c r="H12" s="43">
-        <v>0</v>
-      </c>
-      <c r="I12" s="43">
-        <v>0</v>
-      </c>
-      <c r="J12" s="43">
-        <v>0</v>
-      </c>
-      <c r="K12" s="43">
-        <v>1</v>
-      </c>
-      <c r="L12" s="43" t="s">
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="41">
+        <v>1</v>
+      </c>
+      <c r="E12" s="42">
+        <v>0</v>
+      </c>
+      <c r="F12" s="42">
+        <v>0</v>
+      </c>
+      <c r="G12" s="42">
+        <v>0</v>
+      </c>
+      <c r="H12" s="42">
+        <v>0</v>
+      </c>
+      <c r="I12" s="42">
+        <v>0</v>
+      </c>
+      <c r="J12" s="42">
+        <v>0</v>
+      </c>
+      <c r="K12" s="42">
+        <v>1</v>
+      </c>
+      <c r="L12" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="43">
-        <v>1</v>
-      </c>
-      <c r="N12" s="44">
-        <v>0</v>
-      </c>
-      <c r="O12" s="36">
+      <c r="M12" s="42">
+        <v>1</v>
+      </c>
+      <c r="N12" s="43">
+        <v>0</v>
+      </c>
+      <c r="O12" s="35">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="36">
         <f t="shared" si="0"/>
         <v>6.0606060606060608E-2</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="42">
-        <v>0</v>
-      </c>
-      <c r="D13" s="42">
-        <v>1</v>
-      </c>
-      <c r="E13" s="43">
-        <v>0</v>
-      </c>
-      <c r="F13" s="43">
-        <v>0</v>
-      </c>
-      <c r="G13" s="43">
-        <v>0</v>
-      </c>
-      <c r="H13" s="43">
-        <v>0</v>
-      </c>
-      <c r="I13" s="43">
-        <v>0</v>
-      </c>
-      <c r="J13" s="43">
-        <v>0</v>
-      </c>
-      <c r="K13" s="43">
-        <v>1</v>
-      </c>
-      <c r="L13" s="43">
-        <v>0</v>
-      </c>
-      <c r="M13" s="43" t="s">
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="41">
+        <v>1</v>
+      </c>
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="F13" s="42">
+        <v>0</v>
+      </c>
+      <c r="G13" s="42">
+        <v>0</v>
+      </c>
+      <c r="H13" s="42">
+        <v>0</v>
+      </c>
+      <c r="I13" s="42">
+        <v>0</v>
+      </c>
+      <c r="J13" s="42">
+        <v>0</v>
+      </c>
+      <c r="K13" s="42">
+        <v>1</v>
+      </c>
+      <c r="L13" s="42">
+        <v>0</v>
+      </c>
+      <c r="M13" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="N13" s="44">
-        <v>0</v>
-      </c>
-      <c r="O13" s="36">
+      <c r="N13" s="43">
+        <v>0</v>
+      </c>
+      <c r="O13" s="35">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="P13" s="37">
+      <c r="P13" s="36">
         <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="33">
-        <v>1</v>
-      </c>
-      <c r="D14" s="33">
-        <v>1</v>
-      </c>
-      <c r="E14" s="35">
-        <v>1</v>
-      </c>
-      <c r="F14" s="35">
-        <v>0</v>
-      </c>
-      <c r="G14" s="35">
-        <v>1</v>
-      </c>
-      <c r="H14" s="35">
-        <v>1</v>
-      </c>
-      <c r="I14" s="35">
-        <v>0</v>
-      </c>
-      <c r="J14" s="35">
-        <v>0</v>
-      </c>
-      <c r="K14" s="35">
-        <v>1</v>
-      </c>
-      <c r="L14" s="35">
-        <v>1</v>
-      </c>
-      <c r="M14" s="35">
+      <c r="C14" s="32">
+        <v>1</v>
+      </c>
+      <c r="D14" s="32">
+        <v>1</v>
+      </c>
+      <c r="E14" s="34">
+        <v>1</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0</v>
+      </c>
+      <c r="G14" s="34">
+        <v>1</v>
+      </c>
+      <c r="H14" s="34">
+        <v>1</v>
+      </c>
+      <c r="I14" s="34">
+        <v>0</v>
+      </c>
+      <c r="J14" s="34">
+        <v>0</v>
+      </c>
+      <c r="K14" s="34">
+        <v>1</v>
+      </c>
+      <c r="L14" s="34">
+        <v>1</v>
+      </c>
+      <c r="M14" s="34">
         <v>1</v>
       </c>
       <c r="N14" s="9" t="s">
@@ -3083,21 +3094,21 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
       <c r="O15" s="11">
         <f>SUM(O3:O14)</f>
         <v>66</v>
@@ -3148,8 +3159,8 @@
   </sheetPr>
   <dimension ref="B1:J18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3165,16 +3176,16 @@
       <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="15"/>
@@ -3188,26 +3199,26 @@
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="D3" s="21">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="E3" s="21">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="F3" s="24">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="6">
         <f>D3*C3</f>
-        <v>3.1818181818181821</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="I3" s="6">
         <f>E3*C3</f>
-        <v>3.6363636363636367</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="J3" s="6">
         <f>C3*F3</f>
-        <v>2.2727272727272729</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -3219,26 +3230,26 @@
         <v>1.5151515151515152E-2</v>
       </c>
       <c r="D4" s="22">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="E4" s="22">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="F4" s="25">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="6">
         <f>D4*C4</f>
-        <v>0.90909090909090917</v>
+        <v>7.575757575757576E-2</v>
       </c>
       <c r="I4" s="6">
         <f t="shared" ref="I4:I14" si="0">E4*C4</f>
-        <v>0.75757575757575757</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="J4" s="6">
         <f>C4*F4</f>
-        <v>1.0606060606060606</v>
+        <v>7.575757575757576E-2</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -3250,26 +3261,26 @@
         <v>0.10606060606060606</v>
       </c>
       <c r="D5" s="22">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="E5" s="22">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="F5" s="25">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="6">
         <f t="shared" ref="H5:H14" si="1">D5*C5</f>
-        <v>6.3636363636363642</v>
+        <v>0.53030303030303028</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="0"/>
-        <v>4.2424242424242422</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" ref="J5:J14" si="2">C5*F5</f>
-        <v>4.2424242424242422</v>
+        <v>0.21212121212121213</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -3281,26 +3292,26 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="D6" s="22">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="E6" s="22">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="F6" s="25">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="6">
         <f t="shared" si="1"/>
-        <v>11.666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="0"/>
-        <v>13.333333333333332</v>
+        <v>1</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -3312,26 +3323,26 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="D7" s="22">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="E7" s="22">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="F7" s="25">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="6">
         <f t="shared" si="1"/>
-        <v>7.2727272727272734</v>
+        <v>0.45454545454545459</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="0"/>
-        <v>4.5454545454545459</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="2"/>
-        <v>5.454545454545455</v>
+        <v>0.45454545454545459</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -3343,26 +3354,26 @@
         <v>7.575757575757576E-2</v>
       </c>
       <c r="D8" s="22">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="E8" s="22">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="F8" s="25">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="6">
         <f t="shared" si="1"/>
-        <v>5.6818181818181817</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="0"/>
-        <v>5.3030303030303028</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="2"/>
-        <v>6.0606060606060606</v>
+        <v>0.30303030303030304</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -3374,26 +3385,26 @@
         <v>0.13636363636363635</v>
       </c>
       <c r="D9" s="22">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="E9" s="22">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="F9" s="25">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>8.8636363636363633</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="0"/>
-        <v>7.4999999999999991</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="2"/>
-        <v>6.8181818181818175</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -3405,26 +3416,26 @@
         <v>0.15151515151515152</v>
       </c>
       <c r="D10" s="22">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="E10" s="22">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="F10" s="25">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="6">
         <f t="shared" si="1"/>
-        <v>7.5757575757575761</v>
+        <v>0.90909090909090917</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="0"/>
-        <v>9.0909090909090917</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="2"/>
-        <v>4.5454545454545459</v>
+        <v>0.30303030303030304</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
@@ -3436,13 +3447,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="22">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="E11" s="22">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F11" s="25">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="6">
@@ -3467,26 +3478,26 @@
         <v>6.0606060606060608E-2</v>
       </c>
       <c r="D12" s="22">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E12" s="22">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F12" s="25">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="6">
         <f t="shared" si="1"/>
-        <v>3.6363636363636367</v>
+        <v>0.24242424242424243</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="0"/>
-        <v>1.8181818181818183</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="2"/>
-        <v>5.454545454545455</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
@@ -3498,26 +3509,26 @@
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="D13" s="22">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="E13" s="22">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="F13" s="25">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="6">
         <f t="shared" si="1"/>
-        <v>1.8181818181818183</v>
+        <v>0.15151515151515152</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="0"/>
-        <v>1.8181818181818183</v>
+        <v>0.15151515151515152</v>
       </c>
       <c r="J13" s="6">
         <f t="shared" si="2"/>
-        <v>0.90909090909090917</v>
+        <v>6.0606060606060608E-2</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -3529,44 +3540,44 @@
         <v>0.12121212121212122</v>
       </c>
       <c r="D14" s="23">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="E14" s="23">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="F14" s="26">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="6">
         <f t="shared" si="1"/>
-        <v>8.4848484848484844</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" si="0"/>
-        <v>9.6969696969696972</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="J14" s="6">
         <f t="shared" si="2"/>
-        <v>7.2727272727272734</v>
+        <v>0.24242424242424243</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="29">
+      <c r="C15" s="48"/>
+      <c r="D15" s="28">
         <f>SUM(H3:H14)</f>
-        <v>65.454545454545467</v>
-      </c>
-      <c r="E15" s="28">
+        <v>4.6363636363636367</v>
+      </c>
+      <c r="E15" s="49">
         <f>SUM(I3:I14)</f>
-        <v>61.742424242424249</v>
+        <v>4.0606060606060606</v>
       </c>
       <c r="F15" s="27">
         <f>SUM(J3:J14)</f>
-        <v>49.090909090909086</v>
+        <v>2.9848484848484853</v>
       </c>
       <c r="G15" s="15"/>
     </row>

</xml_diff>